<commit_message>
add report and process data
</commit_message>
<xml_diff>
--- a/漏洞统计.xlsx
+++ b/漏洞统计.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\中科大\大三\编译原理H\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ustc\G3up\BY\Secode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F61CDDE-0AAF-427E-9386-C4766424EB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6FC628-0DEA-40F5-B3BA-7683AC99058B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
   <si>
     <t>Assertion failure</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -284,6 +275,82 @@
   </si>
   <si>
     <t>平均正确率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原漏洞类型（文件夹大类）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实际漏洞类型（实际出现）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1Assertion failure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2Leaking ETH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3Locking ether</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4Reentrancy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5Integer overflow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,3,5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6Unhandled exception</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7Unprotected Delegatecall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8Unprotected Selfdestruct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9Block dependency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,4,5,9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,4,9Transaction order dependency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10Transaction order dependency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,4,6,10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7,10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4889,15 +4956,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5296,27 +5363,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B90" sqref="A86:B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.58203125" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.5546875" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.4140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
     <col min="11" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -5354,7 +5421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5395,7 +5462,7 @@
         <v>258.65379999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -5436,7 +5503,7 @@
         <v>445.60079999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5477,7 +5544,7 @@
         <v>1193.08</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -5518,7 +5585,7 @@
         <v>1214.3109999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -5559,7 +5626,7 @@
         <v>2439.5830000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -5600,7 +5667,7 @@
         <v>1764.729</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -5641,7 +5708,7 @@
         <v>327.86950000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -5682,7 +5749,7 @@
         <v>706.4049</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5723,7 +5790,7 @@
         <v>2791.7330000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D11">
         <f>SUM(D2:D10)</f>
         <v>77</v>
@@ -5749,7 +5816,7 @@
         <v>11141.965</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
         <v>35</v>
       </c>
@@ -5766,7 +5833,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" s="3">
         <f>D11/E11</f>
         <v>0.59230769230769231</v>
@@ -5791,7 +5858,7 @@
         <v>85.707423076923078</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -5808,7 +5875,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -5828,7 +5895,7 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -5848,7 +5915,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -5868,7 +5935,7 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -5888,7 +5955,7 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -5911,7 +5978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -5931,7 +5998,7 @@
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -5951,7 +6018,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -5970,7 +6037,7 @@
       </c>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -5990,7 +6057,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -6010,7 +6077,7 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -6030,7 +6097,7 @@
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26">
         <f>SUM(B15:B25)</f>
         <v>77</v>
@@ -6044,144 +6111,638 @@
         <v>0.58441558441558439</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>51</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B46" t="s">
         <v>60</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C46" t="s">
         <v>57</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D46" t="s">
         <v>58</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E46" t="s">
         <v>52</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F46" t="s">
         <v>59</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>54</v>
       </c>
-      <c r="B63">
+      <c r="B47">
         <v>5</v>
       </c>
-      <c r="C63" s="3">
-        <f>B63/G63</f>
+      <c r="C47" s="3">
+        <f>B47/G47</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="D63" s="3">
-        <f>B63/E63</f>
+      <c r="D47" s="3">
+        <f>B47/E47</f>
         <v>0.17857142857142858</v>
       </c>
-      <c r="E63">
+      <c r="E47">
         <v>28</v>
       </c>
-      <c r="F63" s="3">
-        <f>E63/G63</f>
+      <c r="F47" s="3">
+        <f>E47/G47</f>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G63">
+      <c r="G47">
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>55</v>
       </c>
-      <c r="B64">
+      <c r="B48">
         <v>6</v>
       </c>
-      <c r="C64" s="3">
-        <f>B64/G64</f>
+      <c r="C48" s="3">
+        <f>B48/G48</f>
         <v>0.6</v>
       </c>
-      <c r="D64" s="3">
-        <f>B64/E64</f>
+      <c r="D48" s="3">
+        <f>B48/E48</f>
         <v>0.6</v>
       </c>
-      <c r="E64">
+      <c r="E48">
         <v>10</v>
       </c>
-      <c r="F64" s="3">
-        <f t="shared" ref="F64:F65" si="4">E64/G64</f>
+      <c r="F48" s="3">
+        <f t="shared" ref="F48:F49" si="4">E48/G48</f>
         <v>1</v>
       </c>
-      <c r="G64">
+      <c r="G48">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>56</v>
       </c>
-      <c r="B65">
+      <c r="B49">
         <v>17</v>
       </c>
-      <c r="C65" s="3">
-        <f>B65/G65</f>
+      <c r="C49" s="3">
+        <f>B49/G49</f>
         <v>0.56666666666666665</v>
       </c>
-      <c r="D65" s="3">
-        <f>B65/E65</f>
+      <c r="D49" s="3">
+        <f>B49/E49</f>
         <v>0.85</v>
       </c>
-      <c r="E65">
+      <c r="E49">
         <v>20</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F49" s="3">
         <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G65">
+      <c r="G49">
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B66">
-        <f>SUM(B63:B65)</f>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <f>SUM(B47:B49)</f>
         <v>28</v>
       </c>
-      <c r="E66">
-        <f>SUM(E63:E65)</f>
+      <c r="E50">
+        <f>SUM(E47:E49)</f>
         <v>58</v>
       </c>
-      <c r="G66">
-        <f>SUM(G63:G65)</f>
+      <c r="G50">
+        <f>SUM(G47:G49)</f>
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>61</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C51" t="s">
         <v>62</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E51" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B68" s="3">
-        <f>B66/G66</f>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="3">
+        <f>B50/G50</f>
         <v>0.4</v>
       </c>
-      <c r="C68" s="3">
-        <f>B66/E66</f>
+      <c r="C52" s="3">
+        <f>B50/E50</f>
         <v>0.48275862068965519</v>
       </c>
-      <c r="E68" s="3">
-        <f>E66/G66</f>
+      <c r="E52" s="3">
+        <f>E50/G50</f>
         <v>0.82857142857142863</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>64</v>
+      </c>
+      <c r="B75" t="s">
+        <v>65</v>
+      </c>
+      <c r="E75" t="s">
+        <v>22</v>
+      </c>
+      <c r="F75" t="s">
+        <v>47</v>
+      </c>
+      <c r="H75" t="s">
+        <v>32</v>
+      </c>
+      <c r="J75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>3</v>
+      </c>
+      <c r="F76" s="3">
+        <f>D76/E76</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G76">
+        <v>2</v>
+      </c>
+      <c r="H76" s="3">
+        <f>(E76-G76)/E76</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76" s="3">
+        <f>I76/E76</f>
+        <v>0</v>
+      </c>
+      <c r="K76" s="1">
+        <v>267.41570000000002</v>
+      </c>
+      <c r="L76">
+        <v>258.65379999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>16</v>
+      </c>
+      <c r="B77">
+        <v>6</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77">
+        <v>5</v>
+      </c>
+      <c r="F77" s="3">
+        <f>D77/E77</f>
+        <v>0.4</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77" s="3">
+        <f>(E77-G77)/E77</f>
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>2</v>
+      </c>
+      <c r="J77" s="3">
+        <f t="shared" ref="J77:J84" si="5">I77/E77</f>
+        <v>0.4</v>
+      </c>
+      <c r="K77">
+        <v>469.72410000000002</v>
+      </c>
+      <c r="L77">
+        <v>445.60079999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s">
+        <v>73</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78">
+        <v>11</v>
+      </c>
+      <c r="E78">
+        <v>13</v>
+      </c>
+      <c r="F78" s="3">
+        <f>D78/E78</f>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="G78">
+        <v>5</v>
+      </c>
+      <c r="H78" s="3">
+        <f t="shared" ref="H78:H84" si="6">(E78-G78)/E78</f>
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="I78">
+        <v>6</v>
+      </c>
+      <c r="J78" s="3">
+        <f t="shared" si="5"/>
+        <v>0.46153846153846156</v>
+      </c>
+      <c r="K78">
+        <v>1260.1610000000001</v>
+      </c>
+      <c r="L78">
+        <v>1193.08</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79" t="s">
+        <v>79</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79">
+        <v>11</v>
+      </c>
+      <c r="E79">
+        <v>13</v>
+      </c>
+      <c r="F79" s="3">
+        <f>D79/E79</f>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="G79">
+        <v>2</v>
+      </c>
+      <c r="H79" s="3">
+        <f t="shared" si="6"/>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="I79">
+        <v>9</v>
+      </c>
+      <c r="J79" s="3">
+        <f t="shared" si="5"/>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="K79">
+        <v>1265.269</v>
+      </c>
+      <c r="L79">
+        <v>1214.3109999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" t="s">
+        <v>71</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80">
+        <v>9</v>
+      </c>
+      <c r="E80">
+        <v>29</v>
+      </c>
+      <c r="F80" s="3">
+        <f>D80/E80</f>
+        <v>0.31034482758620691</v>
+      </c>
+      <c r="G80">
+        <v>7</v>
+      </c>
+      <c r="H80" s="3">
+        <f t="shared" si="6"/>
+        <v>0.75862068965517238</v>
+      </c>
+      <c r="I80">
+        <v>2</v>
+      </c>
+      <c r="J80" s="3">
+        <f t="shared" si="5"/>
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="K80">
+        <v>2565.4050000000002</v>
+      </c>
+      <c r="L80">
+        <v>2439.5830000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81">
+        <v>11</v>
+      </c>
+      <c r="E81">
+        <v>21</v>
+      </c>
+      <c r="F81" s="3">
+        <f>D81/E81</f>
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+      <c r="H81" s="3">
+        <f t="shared" si="6"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I81">
+        <v>8</v>
+      </c>
+      <c r="J81" s="3">
+        <f t="shared" si="5"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K81">
+        <v>1851.7929999999999</v>
+      </c>
+      <c r="L81">
+        <v>1764.729</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" t="s">
+        <v>82</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="E82">
+        <v>4</v>
+      </c>
+      <c r="F82" s="3">
+        <f>D82/E82</f>
+        <v>0.75</v>
+      </c>
+      <c r="G82">
+        <v>2</v>
+      </c>
+      <c r="H82" s="3">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82" s="3">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="K82">
+        <v>370.10739999999998</v>
+      </c>
+      <c r="L82">
+        <v>327.86950000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" t="s">
+        <v>72</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D83">
+        <v>5</v>
+      </c>
+      <c r="E83">
+        <v>8</v>
+      </c>
+      <c r="F83" s="3">
+        <f>D83/E83</f>
+        <v>0.625</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>5</v>
+      </c>
+      <c r="J83" s="3">
+        <f t="shared" si="5"/>
+        <v>0.625</v>
+      </c>
+      <c r="K83">
+        <v>726.74789999999996</v>
+      </c>
+      <c r="L83">
+        <v>706.4049</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>27</v>
+      </c>
+      <c r="B84" t="s">
+        <v>78</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D84">
+        <v>23</v>
+      </c>
+      <c r="E84">
+        <v>34</v>
+      </c>
+      <c r="F84" s="3">
+        <f>D84/E84</f>
+        <v>0.67647058823529416</v>
+      </c>
+      <c r="G84">
+        <v>11</v>
+      </c>
+      <c r="H84" s="3">
+        <f t="shared" si="6"/>
+        <v>0.67647058823529416</v>
+      </c>
+      <c r="I84">
+        <v>12</v>
+      </c>
+      <c r="J84" s="3">
+        <f t="shared" si="5"/>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="K84">
+        <v>2917.73</v>
+      </c>
+      <c r="L84">
+        <v>2791.7330000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <f>SUM(D76:D84)</f>
+        <v>77</v>
+      </c>
+      <c r="E85">
+        <f>SUM(E76:E84)</f>
+        <v>130</v>
+      </c>
+      <c r="G85">
+        <f>SUM(G76:G84)</f>
+        <v>32</v>
+      </c>
+      <c r="I85">
+        <f>SUM(I76:I84)</f>
+        <v>45</v>
+      </c>
+      <c r="K85">
+        <f>SUM(K76:K84)</f>
+        <v>11694.353099999998</v>
+      </c>
+      <c r="L85">
+        <f>SUM(L76:L84)</f>
+        <v>11141.965</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>66</v>
+      </c>
+      <c r="B86" t="s">
+        <v>67</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I86" t="s">
+        <v>38</v>
+      </c>
+      <c r="K86" t="s">
+        <v>36</v>
+      </c>
+      <c r="L86" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>68</v>
+      </c>
+      <c r="B87" t="s">
+        <v>69</v>
+      </c>
+      <c r="D87" s="3">
+        <f>D85/E85</f>
+        <v>0.59230769230769231</v>
+      </c>
+      <c r="G87" s="3"/>
+      <c r="I87" s="3">
+        <f>I85/E85</f>
+        <v>0.34615384615384615</v>
+      </c>
+      <c r="J87" t="s">
+        <v>34</v>
+      </c>
+      <c r="K87">
+        <f>K85/E85</f>
+        <v>89.956562307692295</v>
+      </c>
+      <c r="L87">
+        <f>L85/E85</f>
+        <v>85.707423076923078</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>70</v>
+      </c>
+      <c r="B88" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>75</v>
+      </c>
+      <c r="B89" t="s">
+        <v>76</v>
+      </c>
+      <c r="D89" s="3" t="e">
+        <f>D87/E87</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>77</v>
+      </c>
+      <c r="B90" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>